<commit_message>
First working version of batch simulation. Cells persist from one sim to the next, need to fix bug.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tighe/Documents/other/projects/grow algorithm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2678D3BA-FEF5-DC4E-923C-1F57660784D9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046BDF5F-7DDD-524C-9A74-24B5A0C68961}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{C8724D74-C77A-0D4B-AB31-6CDC5376FB0C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{C8724D74-C77A-0D4B-AB31-6CDC5376FB0C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cell Types" sheetId="1" r:id="rId1"/>
+    <sheet name="cell types" sheetId="1" r:id="rId1"/>
+    <sheet name="190824-00" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,34 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Proliferation Rate</t>
-  </si>
-  <si>
-    <t>Metabolism</t>
-  </si>
-  <si>
-    <t>Abundance</t>
-  </si>
-  <si>
-    <t>Food to Move</t>
-  </si>
-  <si>
-    <t>Food to Divide</t>
-  </si>
-  <si>
-    <t>Division Recovery Time</t>
-  </si>
-  <si>
-    <t>Food to Survive</t>
-  </si>
-  <si>
-    <t>Endurance</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>C001</t>
   </si>
@@ -61,6 +35,87 @@
   </si>
   <si>
     <t>C003</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>proliferation rate</t>
+  </si>
+  <si>
+    <t>abundance</t>
+  </si>
+  <si>
+    <t>metabolism</t>
+  </si>
+  <si>
+    <t>food to move</t>
+  </si>
+  <si>
+    <t>food to divide</t>
+  </si>
+  <si>
+    <t>division recovery time</t>
+  </si>
+  <si>
+    <t>food to survive</t>
+  </si>
+  <si>
+    <t>endurance</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>maxIter</t>
+  </si>
+  <si>
+    <t>seeds</t>
+  </si>
+  <si>
+    <t>foodFile</t>
+  </si>
+  <si>
+    <t>mapFile</t>
+  </si>
+  <si>
+    <t>mixRatios</t>
+  </si>
+  <si>
+    <t>outputSize</t>
+  </si>
+  <si>
+    <t>timeWarpFactor</t>
+  </si>
+  <si>
+    <t>foodMaps-04.png</t>
+  </si>
+  <si>
+    <t>foodMaps-00.png</t>
+  </si>
+  <si>
+    <t>C001, C002, C003</t>
+  </si>
+  <si>
+    <t>1, 1, 1</t>
+  </si>
+  <si>
+    <t>2160, 2160</t>
+  </si>
+  <si>
+    <t>S001</t>
+  </si>
+  <si>
+    <t>S002</t>
+  </si>
+  <si>
+    <t>cellTypeNames</t>
+  </si>
+  <si>
+    <t>S003</t>
   </si>
 </sst>
 </file>
@@ -96,8 +151,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +475,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4845CC-ABED-7D41-A78A-6185E27CF326}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -423,18 +486,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -448,7 +511,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -462,7 +525,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -476,7 +539,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -490,55 +553,55 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6">
+        <f>$B$5*4</f>
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <f>$C$5*4</f>
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <f>$D$5*4</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
         <f>$B$5*6</f>
         <v>60</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <f>$C$5*6</f>
         <v>90</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <f>$D$5*6</f>
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <f>$B$5*10</f>
-        <v>100</v>
-      </c>
-      <c r="C7">
-        <f>$C$5*10</f>
-        <v>150</v>
-      </c>
-      <c r="D7">
-        <f>$D$5*10</f>
-        <v>200</v>
-      </c>
-    </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <f>$B$5*1</f>
@@ -555,7 +618,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -570,4 +633,177 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC55BD2-C268-CC4F-83FF-2A0623F23028}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="20.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1">
+        <v>500</v>
+      </c>
+      <c r="C2" s="1">
+        <v>500</v>
+      </c>
+      <c r="D2" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>500</v>
+      </c>
+      <c r="C3" s="1">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C9" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working batch simulator. Excel config file updated with flags when simulation complete. Need to match file names to sim and batch names.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -558,7 +558,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -590,15 +590,11 @@
           <t>completed</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
+      <c r="B2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Updated to fix panadas SettingWithCopy warning
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17540" windowWidth="28800" xWindow="0" yWindow="460"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17540" windowWidth="28800" xWindow="0" yWindow="460"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cell types" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="190824-00" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="190824-01" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -593,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="B2:E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -904,4 +905,225 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="14.6640625"/>
+    <col customWidth="1" max="9" min="2" style="1" width="20.83203125"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>S001</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>S002</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>S003</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>S004</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v/>
+      </c>
+      <c r="D2" t="n">
+        <v/>
+      </c>
+      <c r="E2" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>width</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>height</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>maxIter</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>seeds</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>seedPos</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>center</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>foodFile</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>foodMaps-04.png</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="2" t="n"/>
+      <c r="I8" s="2" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>mapFile</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>foodMaps-00.png</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
+      <c r="F9" s="2" t="n"/>
+      <c r="G9" s="2" t="n"/>
+      <c r="H9" s="2" t="n"/>
+      <c r="I9" s="2" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>cellTypeNames</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>C001</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n"/>
+      <c r="E10" s="2" t="n"/>
+      <c r="F10" s="2" t="n"/>
+      <c r="G10" s="2" t="n"/>
+      <c r="H10" s="2" t="n"/>
+      <c r="I10" s="2" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>mixRatios</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n"/>
+      <c r="D11" s="2" t="n"/>
+      <c r="E11" s="2" t="n"/>
+      <c r="F11" s="2" t="n"/>
+      <c r="G11" s="2" t="n"/>
+      <c r="H11" s="2" t="n"/>
+      <c r="I11" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>outputSize</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>640, 640</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="2" t="n"/>
+      <c r="F12" s="2" t="n"/>
+      <c r="G12" s="2" t="n"/>
+      <c r="H12" s="2" t="n"/>
+      <c r="I12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>timeWarpFactor</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>